<commit_message>
Missed some values in Lincoln2023
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/Lincoln2023.xlsx
+++ b/Tests/Validation/Wheat/Lincoln2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\Validation\Wheat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D603DFF9-76F8-40AC-8971-A30EE93B422F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF828F6-A302-46F8-836F-11A9FAB3807A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1600"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3242,7 +3242,7 @@
         <v>14076.00341297205</v>
       </c>
       <c r="O67">
-        <f t="shared" ref="O67:O117" si="1">N67/1000000</f>
+        <f t="shared" ref="O67:O125" si="1">N67/1000000</f>
         <v>1.4076003412972049E-2</v>
       </c>
       <c r="P67">
@@ -5226,6 +5226,10 @@
       <c r="N119">
         <v>14653.03418520406</v>
       </c>
+      <c r="O119">
+        <f t="shared" si="1"/>
+        <v>1.4653034185204061E-2</v>
+      </c>
       <c r="P119">
         <v>0.10105093476804709</v>
       </c>
@@ -5255,6 +5259,10 @@
       <c r="N120">
         <v>21552.37019774687</v>
       </c>
+      <c r="O120">
+        <f t="shared" si="1"/>
+        <v>2.1552370197746869E-2</v>
+      </c>
       <c r="P120">
         <v>1.0781399703943471</v>
       </c>
@@ -5284,6 +5292,10 @@
       <c r="N121">
         <v>24175.89231706029</v>
       </c>
+      <c r="O121">
+        <f t="shared" si="1"/>
+        <v>2.4175892317060289E-2</v>
+      </c>
       <c r="P121">
         <v>2.5988027768952051</v>
       </c>
@@ -5319,6 +5331,10 @@
       <c r="N122">
         <v>24825.133808260081</v>
       </c>
+      <c r="O122">
+        <f t="shared" si="1"/>
+        <v>2.4825133808260083E-2</v>
+      </c>
       <c r="P122">
         <v>4.0273256338007712</v>
       </c>
@@ -5354,6 +5370,10 @@
       <c r="N123">
         <v>23258.158970633762</v>
       </c>
+      <c r="O123">
+        <f t="shared" si="1"/>
+        <v>2.3258158970633762E-2</v>
+      </c>
       <c r="P123">
         <v>7.0854080958625074</v>
       </c>
@@ -5389,6 +5409,10 @@
       <c r="N124">
         <v>21052.1108653179</v>
       </c>
+      <c r="O124">
+        <f t="shared" si="1"/>
+        <v>2.10521108653179E-2</v>
+      </c>
       <c r="P124">
         <v>5.9431640487927346</v>
       </c>
@@ -5423,6 +5447,10 @@
       </c>
       <c r="N125">
         <v>17649.933018694359</v>
+      </c>
+      <c r="O125">
+        <f t="shared" si="1"/>
+        <v>1.7649933018694358E-2</v>
       </c>
       <c r="P125">
         <v>3.9110316660716942</v>

</xml_diff>